<commit_message>
Added chart to results
added jpg to readme as well
</commit_message>
<xml_diff>
--- a/matrix_multiplication/results.xlsx
+++ b/matrix_multiplication/results.xlsx
@@ -115,6 +115,1813 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Measured matrix multiplication time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>using_intel_compiler!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sequential Two-dim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="9BBB59">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.106999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>using_intel_compiler!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sequential Single-dim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="1F497D">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.161000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>using_intel_compiler!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Str-Single-Dim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1689999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.916599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>using_intel_compiler!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Str-Quad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55159999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8437999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.2502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>using_intel_compiler!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Str-Single-Dim-SIMD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.46E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5399999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8719999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.943999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>using_intel_compiler!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Str-Quad-SIMD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.114</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0600000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0490000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.4344</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="420255960"/>
+        <c:axId val="420257136"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>using_intel_compiler!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strassen-Wiki</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>using_intel_compiler!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7799999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46079999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1907999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.067399999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145.06100000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="420256352"/>
+        <c:axId val="420256744"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="420255960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Matrix row size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420257136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="420257136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>execution time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420255960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="420256744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="420256352"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="420256352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="420256744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,11 +2185,265 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -477,7 +2538,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A11" si="0">A3*2</f>
+        <f t="shared" ref="A4:A10" si="0">A3*2</f>
         <v>64</v>
       </c>
       <c r="B4" s="2">
@@ -665,5 +2726,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>